<commit_message>
replication data for paper
</commit_message>
<xml_diff>
--- a/hdb data (standardised).xlsx
+++ b/hdb data (standardised).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EilyTan/Desktop/dizzy/Submission file/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EilyTan/Documents/GitHub/lsedizzy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3D38442-BC75-034C-AE77-191538838BD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E88B8EB-7EF5-8E4A-91E6-C1E4A9842146}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2920" yWindow="1520" windowWidth="25880" windowHeight="16480" xr2:uid="{B15FD220-2804-1945-9359-894F3E26F788}"/>
   </bookViews>
@@ -401,7 +401,7 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>